<commit_message>
Updates to EFM app - adding new graphics
</commit_message>
<xml_diff>
--- a/EFM_shiny (1).xlsx
+++ b/EFM_shiny (1).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/018fd3f915004678/Documents/GitHub/EFMDataScripts_Lily/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_26E0AAB5AAA6581E828C46975CE7567F29EA0B52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2138DEE-BFDA-4043-A603-B3C9EB4FDB8E}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" tabRatio="971" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="971" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -158,9 +164,6 @@
     <t>rp-contact-field.app_launch_history</t>
   </si>
   <si>
-    <t>text = "Max Days Btwn  App Launches", colour = "blue"</t>
-  </si>
-  <si>
     <t>rp-contact-field.max_days_between_app_launches</t>
   </si>
   <si>
@@ -176,9 +179,6 @@
     <t>text = "Button Click History", colour = "blue"</t>
   </si>
   <si>
-    <t>rp-contact-field.activities_button_click_history</t>
-  </si>
-  <si>
     <t>box2</t>
   </si>
   <si>
@@ -197,9 +197,6 @@
     <t>rp-contact-field.has_accessed_activities</t>
   </si>
   <si>
-    <t>rp-contact-field.storybooks_button_click_history</t>
-  </si>
-  <si>
     <t>text = "Storybook Button Click History", colour = "blue"</t>
   </si>
   <si>
@@ -243,19 +240,52 @@
   </si>
   <si>
     <t>plhdata_org</t>
+  </si>
+  <si>
+    <t>data_manip</t>
+  </si>
+  <si>
+    <t>graph_manip</t>
+  </si>
+  <si>
+    <t>bar_freq</t>
+  </si>
+  <si>
+    <t>text = "App Language", colour = "blue"</t>
+  </si>
+  <si>
+    <t>rp-contact-field._app_language</t>
+  </si>
+  <si>
+    <t>specify_plot</t>
+  </si>
+  <si>
+    <t>text = "App Last Launch", colour = "blue"</t>
+  </si>
+  <si>
+    <t>%&gt;% filter(!is.na(app_last_launch)) %&gt;% group_by(app_last_launch) %&gt;% summarise(frequency = n())</t>
+  </si>
+  <si>
+    <t>geom_line(aes(x = app_last_launch, y = frequency)) + geom_point(aes(x = app_last_launch, y = frequency)) + labs(x = "Date", y = "Frequency", title = "Frequency of Values by Date")</t>
+  </si>
+  <si>
+    <t>text = "Max Days Btwn App Launches", colour = "blue"</t>
+  </si>
+  <si>
+    <t>rp-contact-field.activities_button_click_history_count</t>
+  </si>
+  <si>
+    <t>rp-contact-field.storybooks_button_click_history_count</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,346 +325,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -642,253 +342,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -896,64 +354,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1240,24 +653,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.8190476190476" customWidth="1"/>
-    <col min="2" max="2" width="16.1809523809524" customWidth="1"/>
-    <col min="3" max="3" width="16.2666666666667" customWidth="1"/>
-    <col min="4" max="4" width="20.4571428571429" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1317,41 +730,39 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.8190476190476" customWidth="1"/>
-    <col min="2" max="2" width="13.8190476190476" customWidth="1"/>
-    <col min="3" max="3" width="78.1809523809524" customWidth="1"/>
-    <col min="4" max="4" width="36.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="15.1809523809524" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="78.1796875" customWidth="1"/>
+    <col min="4" max="4" width="36.26953125" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1371,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1455,31 +866,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.57142857142857" customWidth="1"/>
-    <col min="2" max="2" width="12.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="51.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="26.2095238095238" customWidth="1"/>
-    <col min="6" max="6" width="15.1809523809524" customWidth="1"/>
+    <col min="4" max="4" width="51.453125" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1490,132 +899,173 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="G2">
+      <c r="I2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6">
+      <c r="I8">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.5428571428571" customWidth="1"/>
-    <col min="2" max="2" width="6.54285714285714" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="53.5428571428571" customWidth="1"/>
-    <col min="5" max="5" width="51.1809523809524" customWidth="1"/>
-    <col min="6" max="6" width="12.9047619047619" customWidth="1"/>
-    <col min="7" max="7" width="15.1809523809524" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="51.1796875" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1646,16 +1096,16 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3"/>
       <c r="H2">
@@ -1667,16 +1117,16 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1687,16 +1137,16 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1704,32 +1154,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.5428571428571" customWidth="1"/>
-    <col min="2" max="2" width="6.54285714285714" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="53.5428571428571" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
     <col min="5" max="5" width="73" customWidth="1"/>
-    <col min="6" max="6" width="12.9047619047619" customWidth="1"/>
-    <col min="7" max="7" width="15.1809523809524" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1760,16 +1208,16 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F2" s="3"/>
       <c r="H2">
@@ -1778,19 +1226,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1801,16 +1249,16 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -1821,16 +1269,16 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1838,24 +1286,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.1809523809524" customWidth="1"/>
-    <col min="2" max="2" width="19.4571428571429" customWidth="1"/>
-    <col min="3" max="3" width="12.8190476190476" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1869,17 +1315,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1887,25 +1333,24 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>